<commit_message>
Plasteel Surgery (Continued) 업데이트
#326
</commit_message>
<xml_diff>
--- a/Data/Mlie/Plasteel Surgery (Continued) - 2018276375/2018276375.xlsx
+++ b/Data/Mlie/Plasteel Surgery (Continued) - 2018276375/2018276375.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\Plasteel Surgery (Continued) - 2018276375\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\Plasteel.Surgery.Continued.-.2018276375.-.Korean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8460F8E6-609E-470C-864D-A7CFDAEE0945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76611D2A-9DE7-4BBF-A0DB-D4B9F828ADB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main" sheetId="1" r:id="rId1"/>
-    <sheet name="Merge" sheetId="2" r:id="rId2"/>
+    <sheet name="Main_231220" sheetId="3" r:id="rId1"/>
+    <sheet name="231211" sheetId="1" r:id="rId2"/>
+    <sheet name="Merge" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="257">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -809,6 +810,28 @@
   </si>
   <si>
     <t>성형수술 중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체형 변경</t>
+  </si>
+  <si>
+    <t>성전환</t>
+  </si>
+  <si>
+    <t>안면 성형</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0}(은)는 {1}의 {2} 수술을 완벽하게 성공시켰습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0}(은)는 {1}의 {2} 수술을 실패했습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>음성</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1179,10 +1202,1179 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A78166E-45CE-4937-84EA-7E4530326BE3}">
+  <dimension ref="A1:F67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="53.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.83203125" customWidth="1"/>
+    <col min="5" max="5" width="67.08203125" customWidth="1"/>
+    <col min="6" max="6" width="39.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A39" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A41" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A44" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A45" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A46" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A47" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A48" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A49" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A50" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A51" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A52" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A53" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A54" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A55" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A56" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A57" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A58" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A59" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A60" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A61" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A62" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A63" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A64" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A65" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A66" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A67" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -2600,7 +3792,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B92D5E44-6E40-4CD3-B87B-A837D39CD2F3}">
   <dimension ref="C2:E66"/>
   <sheetViews>
@@ -2622,7 +3814,7 @@
         <v>182</v>
       </c>
       <c r="E2">
-        <f>MATCH(C2,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C2,'231211'!$A$2:$A$67,0)</f>
         <v>60</v>
       </c>
     </row>
@@ -2634,7 +3826,7 @@
         <v>183</v>
       </c>
       <c r="E3">
-        <f>MATCH(C3,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C3,'231211'!$A$2:$A$67,0)</f>
         <v>61</v>
       </c>
     </row>
@@ -2646,7 +3838,7 @@
         <v>184</v>
       </c>
       <c r="E4">
-        <f>MATCH(C4,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C4,'231211'!$A$2:$A$67,0)</f>
         <v>62</v>
       </c>
     </row>
@@ -2658,7 +3850,7 @@
         <v>185</v>
       </c>
       <c r="E5">
-        <f>MATCH(C5,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C5,'231211'!$A$2:$A$67,0)</f>
         <v>63</v>
       </c>
     </row>
@@ -2670,7 +3862,7 @@
         <v>186</v>
       </c>
       <c r="E6">
-        <f>MATCH(C6,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C6,'231211'!$A$2:$A$67,0)</f>
         <v>64</v>
       </c>
     </row>
@@ -2682,7 +3874,7 @@
         <v>187</v>
       </c>
       <c r="E7">
-        <f>MATCH(C7,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C7,'231211'!$A$2:$A$67,0)</f>
         <v>65</v>
       </c>
     </row>
@@ -2694,7 +3886,7 @@
         <v>188</v>
       </c>
       <c r="E8">
-        <f>MATCH(C8,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C8,'231211'!$A$2:$A$67,0)</f>
         <v>66</v>
       </c>
     </row>
@@ -2706,7 +3898,7 @@
         <v>189</v>
       </c>
       <c r="E9">
-        <f>MATCH(C9,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C9,'231211'!$A$2:$A$67,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -2718,7 +3910,7 @@
         <v>190</v>
       </c>
       <c r="E10">
-        <f>MATCH(C10,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C10,'231211'!$A$2:$A$67,0)</f>
         <v>3</v>
       </c>
     </row>
@@ -2730,7 +3922,7 @@
         <v>191</v>
       </c>
       <c r="E11">
-        <f>MATCH(C11,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C11,'231211'!$A$2:$A$67,0)</f>
         <v>4</v>
       </c>
     </row>
@@ -2742,7 +3934,7 @@
         <v>192</v>
       </c>
       <c r="E12">
-        <f>MATCH(C12,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C12,'231211'!$A$2:$A$67,0)</f>
         <v>5</v>
       </c>
     </row>
@@ -2754,7 +3946,7 @@
         <v>193</v>
       </c>
       <c r="E13">
-        <f>MATCH(C13,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C13,'231211'!$A$2:$A$67,0)</f>
         <v>6</v>
       </c>
     </row>
@@ -2766,7 +3958,7 @@
         <v>194</v>
       </c>
       <c r="E14">
-        <f>MATCH(C14,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C14,'231211'!$A$2:$A$67,0)</f>
         <v>7</v>
       </c>
     </row>
@@ -2778,7 +3970,7 @@
         <v>195</v>
       </c>
       <c r="E15">
-        <f>MATCH(C15,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C15,'231211'!$A$2:$A$67,0)</f>
         <v>8</v>
       </c>
     </row>
@@ -2790,7 +3982,7 @@
         <v>196</v>
       </c>
       <c r="E16">
-        <f>MATCH(C16,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C16,'231211'!$A$2:$A$67,0)</f>
         <v>10</v>
       </c>
     </row>
@@ -2802,7 +3994,7 @@
         <v>197</v>
       </c>
       <c r="E17">
-        <f>MATCH(C17,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C17,'231211'!$A$2:$A$67,0)</f>
         <v>11</v>
       </c>
     </row>
@@ -2814,7 +4006,7 @@
         <v>198</v>
       </c>
       <c r="E18">
-        <f>MATCH(C18,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C18,'231211'!$A$2:$A$67,0)</f>
         <v>9</v>
       </c>
     </row>
@@ -2826,7 +4018,7 @@
         <v>199</v>
       </c>
       <c r="E19">
-        <f>MATCH(C19,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C19,'231211'!$A$2:$A$67,0)</f>
         <v>13</v>
       </c>
     </row>
@@ -2838,7 +4030,7 @@
         <v>200</v>
       </c>
       <c r="E20">
-        <f>MATCH(C20,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C20,'231211'!$A$2:$A$67,0)</f>
         <v>14</v>
       </c>
     </row>
@@ -2850,7 +4042,7 @@
         <v>198</v>
       </c>
       <c r="E21">
-        <f>MATCH(C21,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C21,'231211'!$A$2:$A$67,0)</f>
         <v>12</v>
       </c>
     </row>
@@ -2862,7 +4054,7 @@
         <v>201</v>
       </c>
       <c r="E22">
-        <f>MATCH(C22,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C22,'231211'!$A$2:$A$67,0)</f>
         <v>16</v>
       </c>
     </row>
@@ -2874,7 +4066,7 @@
         <v>202</v>
       </c>
       <c r="E23">
-        <f>MATCH(C23,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C23,'231211'!$A$2:$A$67,0)</f>
         <v>17</v>
       </c>
     </row>
@@ -2886,7 +4078,7 @@
         <v>198</v>
       </c>
       <c r="E24">
-        <f>MATCH(C24,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C24,'231211'!$A$2:$A$67,0)</f>
         <v>15</v>
       </c>
     </row>
@@ -2898,7 +4090,7 @@
         <v>203</v>
       </c>
       <c r="E25">
-        <f>MATCH(C25,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C25,'231211'!$A$2:$A$67,0)</f>
         <v>19</v>
       </c>
     </row>
@@ -2910,7 +4102,7 @@
         <v>204</v>
       </c>
       <c r="E26">
-        <f>MATCH(C26,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C26,'231211'!$A$2:$A$67,0)</f>
         <v>20</v>
       </c>
     </row>
@@ -2922,7 +4114,7 @@
         <v>198</v>
       </c>
       <c r="E27">
-        <f>MATCH(C27,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C27,'231211'!$A$2:$A$67,0)</f>
         <v>18</v>
       </c>
     </row>
@@ -2934,7 +4126,7 @@
         <v>205</v>
       </c>
       <c r="E28">
-        <f>MATCH(C28,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C28,'231211'!$A$2:$A$67,0)</f>
         <v>22</v>
       </c>
     </row>
@@ -2946,7 +4138,7 @@
         <v>206</v>
       </c>
       <c r="E29">
-        <f>MATCH(C29,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C29,'231211'!$A$2:$A$67,0)</f>
         <v>23</v>
       </c>
     </row>
@@ -2958,7 +4150,7 @@
         <v>198</v>
       </c>
       <c r="E30">
-        <f>MATCH(C30,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C30,'231211'!$A$2:$A$67,0)</f>
         <v>21</v>
       </c>
     </row>
@@ -2970,7 +4162,7 @@
         <v>207</v>
       </c>
       <c r="E31">
-        <f>MATCH(C31,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C31,'231211'!$A$2:$A$67,0)</f>
         <v>25</v>
       </c>
     </row>
@@ -2982,7 +4174,7 @@
         <v>208</v>
       </c>
       <c r="E32">
-        <f>MATCH(C32,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C32,'231211'!$A$2:$A$67,0)</f>
         <v>26</v>
       </c>
     </row>
@@ -2994,7 +4186,7 @@
         <v>198</v>
       </c>
       <c r="E33">
-        <f>MATCH(C33,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C33,'231211'!$A$2:$A$67,0)</f>
         <v>24</v>
       </c>
     </row>
@@ -3006,7 +4198,7 @@
         <v>209</v>
       </c>
       <c r="E34">
-        <f>MATCH(C34,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C34,'231211'!$A$2:$A$67,0)</f>
         <v>28</v>
       </c>
     </row>
@@ -3018,7 +4210,7 @@
         <v>210</v>
       </c>
       <c r="E35">
-        <f>MATCH(C35,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C35,'231211'!$A$2:$A$67,0)</f>
         <v>29</v>
       </c>
     </row>
@@ -3030,7 +4222,7 @@
         <v>198</v>
       </c>
       <c r="E36">
-        <f>MATCH(C36,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C36,'231211'!$A$2:$A$67,0)</f>
         <v>27</v>
       </c>
     </row>
@@ -3042,7 +4234,7 @@
         <v>211</v>
       </c>
       <c r="E37">
-        <f>MATCH(C37,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C37,'231211'!$A$2:$A$67,0)</f>
         <v>30</v>
       </c>
     </row>
@@ -3054,7 +4246,7 @@
         <v>212</v>
       </c>
       <c r="E38">
-        <f>MATCH(C38,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C38,'231211'!$A$2:$A$67,0)</f>
         <v>31</v>
       </c>
     </row>
@@ -3066,7 +4258,7 @@
         <v>198</v>
       </c>
       <c r="E39">
-        <f>MATCH(C39,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C39,'231211'!$A$2:$A$67,0)</f>
         <v>32</v>
       </c>
     </row>
@@ -3078,7 +4270,7 @@
         <v>213</v>
       </c>
       <c r="E40">
-        <f>MATCH(C40,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C40,'231211'!$A$2:$A$67,0)</f>
         <v>33</v>
       </c>
     </row>
@@ -3090,7 +4282,7 @@
         <v>212</v>
       </c>
       <c r="E41">
-        <f>MATCH(C41,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C41,'231211'!$A$2:$A$67,0)</f>
         <v>34</v>
       </c>
     </row>
@@ -3102,7 +4294,7 @@
         <v>198</v>
       </c>
       <c r="E42">
-        <f>MATCH(C42,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C42,'231211'!$A$2:$A$67,0)</f>
         <v>35</v>
       </c>
     </row>
@@ -3114,7 +4306,7 @@
         <v>215</v>
       </c>
       <c r="E43">
-        <f>MATCH(C43,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C43,'231211'!$A$2:$A$67,0)</f>
         <v>36</v>
       </c>
     </row>
@@ -3126,7 +4318,7 @@
         <v>212</v>
       </c>
       <c r="E44">
-        <f>MATCH(C44,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C44,'231211'!$A$2:$A$67,0)</f>
         <v>37</v>
       </c>
     </row>
@@ -3138,7 +4330,7 @@
         <v>198</v>
       </c>
       <c r="E45">
-        <f>MATCH(C45,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C45,'231211'!$A$2:$A$67,0)</f>
         <v>38</v>
       </c>
     </row>
@@ -3150,7 +4342,7 @@
         <v>217</v>
       </c>
       <c r="E46">
-        <f>MATCH(C46,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C46,'231211'!$A$2:$A$67,0)</f>
         <v>39</v>
       </c>
     </row>
@@ -3162,7 +4354,7 @@
         <v>218</v>
       </c>
       <c r="E47">
-        <f>MATCH(C47,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C47,'231211'!$A$2:$A$67,0)</f>
         <v>40</v>
       </c>
     </row>
@@ -3174,7 +4366,7 @@
         <v>198</v>
       </c>
       <c r="E48">
-        <f>MATCH(C48,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C48,'231211'!$A$2:$A$67,0)</f>
         <v>41</v>
       </c>
     </row>
@@ -3186,7 +4378,7 @@
         <v>220</v>
       </c>
       <c r="E49">
-        <f>MATCH(C49,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C49,'231211'!$A$2:$A$67,0)</f>
         <v>42</v>
       </c>
     </row>
@@ -3198,7 +4390,7 @@
         <v>218</v>
       </c>
       <c r="E50">
-        <f>MATCH(C50,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C50,'231211'!$A$2:$A$67,0)</f>
         <v>43</v>
       </c>
     </row>
@@ -3210,7 +4402,7 @@
         <v>198</v>
       </c>
       <c r="E51">
-        <f>MATCH(C51,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C51,'231211'!$A$2:$A$67,0)</f>
         <v>44</v>
       </c>
     </row>
@@ -3222,7 +4414,7 @@
         <v>222</v>
       </c>
       <c r="E52">
-        <f>MATCH(C52,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C52,'231211'!$A$2:$A$67,0)</f>
         <v>46</v>
       </c>
     </row>
@@ -3234,7 +4426,7 @@
         <v>223</v>
       </c>
       <c r="E53">
-        <f>MATCH(C53,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C53,'231211'!$A$2:$A$67,0)</f>
         <v>47</v>
       </c>
     </row>
@@ -3246,7 +4438,7 @@
         <v>224</v>
       </c>
       <c r="E54">
-        <f>MATCH(C54,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C54,'231211'!$A$2:$A$67,0)</f>
         <v>48</v>
       </c>
     </row>
@@ -3258,7 +4450,7 @@
         <v>225</v>
       </c>
       <c r="E55">
-        <f>MATCH(C55,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C55,'231211'!$A$2:$A$67,0)</f>
         <v>49</v>
       </c>
     </row>
@@ -3270,7 +4462,7 @@
         <v>226</v>
       </c>
       <c r="E56">
-        <f>MATCH(C56,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C56,'231211'!$A$2:$A$67,0)</f>
         <v>50</v>
       </c>
     </row>
@@ -3282,7 +4474,7 @@
         <v>227</v>
       </c>
       <c r="E57">
-        <f>MATCH(C57,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C57,'231211'!$A$2:$A$67,0)</f>
         <v>51</v>
       </c>
     </row>
@@ -3294,7 +4486,7 @@
         <v>228</v>
       </c>
       <c r="E58">
-        <f>MATCH(C58,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C58,'231211'!$A$2:$A$67,0)</f>
         <v>52</v>
       </c>
     </row>
@@ -3306,7 +4498,7 @@
         <v>229</v>
       </c>
       <c r="E59">
-        <f>MATCH(C59,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C59,'231211'!$A$2:$A$67,0)</f>
         <v>53</v>
       </c>
     </row>
@@ -3318,7 +4510,7 @@
         <v>230</v>
       </c>
       <c r="E60">
-        <f>MATCH(C60,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C60,'231211'!$A$2:$A$67,0)</f>
         <v>54</v>
       </c>
     </row>
@@ -3330,7 +4522,7 @@
         <v>231</v>
       </c>
       <c r="E61">
-        <f>MATCH(C61,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C61,'231211'!$A$2:$A$67,0)</f>
         <v>55</v>
       </c>
     </row>
@@ -3342,7 +4534,7 @@
         <v>190</v>
       </c>
       <c r="E62">
-        <f>MATCH(C62,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C62,'231211'!$A$2:$A$67,0)</f>
         <v>56</v>
       </c>
     </row>
@@ -3354,7 +4546,7 @@
         <v>191</v>
       </c>
       <c r="E63">
-        <f>MATCH(C63,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C63,'231211'!$A$2:$A$67,0)</f>
         <v>57</v>
       </c>
     </row>
@@ -3366,7 +4558,7 @@
         <v>232</v>
       </c>
       <c r="E64">
-        <f>MATCH(C64,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C64,'231211'!$A$2:$A$67,0)</f>
         <v>58</v>
       </c>
     </row>
@@ -3378,7 +4570,7 @@
         <v>233</v>
       </c>
       <c r="E65">
-        <f>MATCH(C65,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C65,'231211'!$A$2:$A$67,0)</f>
         <v>59</v>
       </c>
     </row>
@@ -3390,7 +4582,7 @@
         <v>234</v>
       </c>
       <c r="E66">
-        <f>MATCH(C66,Main!$A$2:$A$67,0)</f>
+        <f>MATCH(C66,'231211'!$A$2:$A$67,0)</f>
         <v>45</v>
       </c>
     </row>

</xml_diff>